<commit_message>
Invalid SignUp with two negative scenarios
</commit_message>
<xml_diff>
--- a/Data/BTInvalidSignUp.xlsx
+++ b/Data/BTInvalidSignUp.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jisha\git\BetterThat\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3E5F6A58-EF14-40E9-87F0-7191F0B8DDA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B8D24C1-5FB6-4B11-BE35-2A6F631D55D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4788" yWindow="4608" windowWidth="18492" windowHeight="13512" xr2:uid="{F5B428EB-3013-412F-A92D-21EF19963307}"/>
+    <workbookView xWindow="4548" yWindow="168" windowWidth="18492" windowHeight="13512" xr2:uid="{F5B428EB-3013-412F-A92D-21EF19963307}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Invalid_SignUp _Data" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Email ID</t>
   </si>
@@ -37,6 +37,18 @@
   </si>
   <si>
     <t>Password</t>
+  </si>
+  <si>
+    <t>testnum123@yopmail.com</t>
+  </si>
+  <si>
+    <t>Jis</t>
+  </si>
+  <si>
+    <t>Jay</t>
+  </si>
+  <si>
+    <t>abcd</t>
   </si>
 </sst>
 </file>
@@ -399,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC0C6159-6A61-4A1C-A71B-D01839E28386}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -427,10 +439,37 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
-      <c r="D2" s="1"/>
+      <c r="A2">
+        <v>123</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1" xr:uid="{9ED8C3B4-D463-43D2-9A75-34D570ECCE53}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
New updated scripts 10th May
</commit_message>
<xml_diff>
--- a/Data/BTInvalidSignUp.xlsx
+++ b/Data/BTInvalidSignUp.xlsx
@@ -3,19 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jisha\git\BetterThat\Data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B8D24C1-5FB6-4B11-BE35-2A6F631D55D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{007C215D-750D-4BD6-BA7A-37CBED30AAD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4548" yWindow="168" windowWidth="18492" windowHeight="13512" xr2:uid="{F5B428EB-3013-412F-A92D-21EF19963307}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{F5B428EB-3013-412F-A92D-21EF19963307}"/>
   </bookViews>
   <sheets>
     <sheet name="Invalid_SignUp _Data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>Email ID</t>
   </si>
@@ -39,9 +35,6 @@
     <t>Password</t>
   </si>
   <si>
-    <t>testnum123@yopmail.com</t>
-  </si>
-  <si>
     <t>Jis</t>
   </si>
   <si>
@@ -49,6 +42,15 @@
   </si>
   <si>
     <t>abcd</t>
+  </si>
+  <si>
+    <t>testnum456@yopmail.com</t>
+  </si>
+  <si>
+    <t>testnum12@yopmail.com</t>
+  </si>
+  <si>
+    <t>BT@2021</t>
   </si>
 </sst>
 </file>
@@ -411,10 +413,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC0C6159-6A61-4A1C-A71B-D01839E28386}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -454,21 +456,37 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" t="s">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1" xr:uid="{9ED8C3B4-D463-43D2-9A75-34D570ECCE53}"/>
+    <hyperlink ref="A4" r:id="rId2" xr:uid="{E5FE6760-1A88-4106-AAC9-555C052EE417}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{CA9B18A6-3ED8-4CDA-9E88-CE10ADC64AED}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>